<commit_message>
SF 총 Equip6001 추가
</commit_message>
<xml_diff>
--- a/Excel/Equip.xlsx
+++ b/Excel/Equip.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{564D1A98-E116-4F70-9A48-0839097003EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34542986-DFA3-433E-B39C-A24BAD60ECE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{744FAB8B-2B4C-47C4-9B52-EAF29B7E3396}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{744FAB8B-2B4C-47C4-9B52-EAF29B7E3396}"/>
   </bookViews>
   <sheets>
     <sheet name="EquipTable" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="195">
   <si>
     <t>Equip0001</t>
   </si>
@@ -611,6 +611,15 @@
   </si>
   <si>
     <t>EquipName_StrongMaul</t>
+  </si>
+  <si>
+    <t>SciFiWarriorGun</t>
+  </si>
+  <si>
+    <t>Shot_SciFiWarriorGun</t>
+  </si>
+  <si>
+    <t>EquipName_SciFiWarriorGun</t>
   </si>
 </sst>
 </file>
@@ -3631,6 +3640,15 @@
       <c r="J80">
         <v>0</v>
       </c>
+      <c r="L80" t="s">
+        <v>192</v>
+      </c>
+      <c r="M80" t="s">
+        <v>193</v>
+      </c>
+      <c r="N80" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" t="s">

</xml_diff>

<commit_message>
innergrade => innerGrade 컬럼명 수정
</commit_message>
<xml_diff>
--- a/Excel/Equip.xlsx
+++ b/Excel/Equip.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01AE0723-E700-4FC9-8137-E8AA18236767}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84595B73-403D-4CEB-AB4A-8E44B34BDBD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{744FAB8B-2B4C-47C4-9B52-EAF29B7E3396}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{744FAB8B-2B4C-47C4-9B52-EAF29B7E3396}"/>
   </bookViews>
   <sheets>
     <sheet name="EquipTable" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="199">
   <si>
     <t>Equip0001</t>
   </si>
@@ -127,9 +127,6 @@
   </si>
   <si>
     <t>multi|Float</t>
-  </si>
-  <si>
-    <t>innergrade|Int</t>
   </si>
   <si>
     <t>optionType|Int</t>
@@ -1002,8 +999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{314FDFEB-84DC-4FDB-9708-1D7DBC9715D5}">
   <dimension ref="A1:N118"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="A100" sqref="A100"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1022,10 +1019,10 @@
         <v>24</v>
       </c>
       <c r="D1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1" t="s">
         <v>31</v>
-      </c>
-      <c r="E1" t="s">
-        <v>32</v>
       </c>
       <c r="F1" t="s">
         <v>25</v>
@@ -1037,22 +1034,22 @@
         <v>27</v>
       </c>
       <c r="I1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J1" t="s">
         <v>28</v>
       </c>
       <c r="K1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L1" t="s">
+        <v>110</v>
+      </c>
+      <c r="M1" t="s">
         <v>111</v>
       </c>
-      <c r="M1" t="s">
-        <v>112</v>
-      </c>
       <c r="N1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -1087,18 +1084,18 @@
         <v>0</v>
       </c>
       <c r="L2" t="s">
+        <v>113</v>
+      </c>
+      <c r="M2" t="s">
+        <v>112</v>
+      </c>
+      <c r="N2" t="s">
         <v>114</v>
-      </c>
-      <c r="M2" t="s">
-        <v>113</v>
-      </c>
-      <c r="N2" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1128,13 +1125,13 @@
         <v>0</v>
       </c>
       <c r="L3" t="s">
+        <v>145</v>
+      </c>
+      <c r="M3" t="s">
         <v>146</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>147</v>
-      </c>
-      <c r="N3" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
@@ -1169,18 +1166,18 @@
         <v>0</v>
       </c>
       <c r="L4" t="s">
+        <v>154</v>
+      </c>
+      <c r="M4" t="s">
         <v>155</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>156</v>
-      </c>
-      <c r="N4" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1530,18 +1527,18 @@
         <v>0</v>
       </c>
       <c r="L15" t="s">
+        <v>148</v>
+      </c>
+      <c r="M15" t="s">
         <v>149</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>150</v>
-      </c>
-      <c r="N15" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1571,13 +1568,13 @@
         <v>0</v>
       </c>
       <c r="L16" t="s">
+        <v>175</v>
+      </c>
+      <c r="M16" t="s">
         <v>176</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>177</v>
-      </c>
-      <c r="N16" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -1614,7 +1611,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -1934,7 +1931,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28">
         <v>2</v>
@@ -1966,7 +1963,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B29">
         <v>2</v>
@@ -1998,7 +1995,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B30">
         <v>2</v>
@@ -2030,7 +2027,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -2062,7 +2059,7 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B32">
         <v>2</v>
@@ -2094,7 +2091,7 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B33">
         <v>2</v>
@@ -2126,7 +2123,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B34">
         <v>2</v>
@@ -2156,18 +2153,18 @@
         <v>0</v>
       </c>
       <c r="L34" t="s">
+        <v>169</v>
+      </c>
+      <c r="M34" t="s">
         <v>170</v>
       </c>
-      <c r="M34" t="s">
+      <c r="N34" t="s">
         <v>171</v>
-      </c>
-      <c r="N34" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B35">
         <v>2</v>
@@ -2199,7 +2196,7 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -2231,7 +2228,7 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B37">
         <v>2</v>
@@ -2263,7 +2260,7 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B38">
         <v>2</v>
@@ -2295,7 +2292,7 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B39">
         <v>2</v>
@@ -2327,7 +2324,7 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B40">
         <v>2</v>
@@ -2359,7 +2356,7 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B41">
         <v>3</v>
@@ -2391,7 +2388,7 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B42">
         <v>3</v>
@@ -2423,7 +2420,7 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B43">
         <v>3</v>
@@ -2455,7 +2452,7 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B44">
         <v>3</v>
@@ -2487,7 +2484,7 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B45">
         <v>3</v>
@@ -2517,18 +2514,18 @@
         <v>0</v>
       </c>
       <c r="L45" t="s">
+        <v>166</v>
+      </c>
+      <c r="M45" t="s">
         <v>167</v>
       </c>
-      <c r="M45" t="s">
+      <c r="N45" t="s">
         <v>168</v>
-      </c>
-      <c r="N45" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B46">
         <v>3</v>
@@ -2560,7 +2557,7 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B47">
         <v>3</v>
@@ -2592,7 +2589,7 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B48">
         <v>3</v>
@@ -2624,7 +2621,7 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B49">
         <v>3</v>
@@ -2656,7 +2653,7 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B50">
         <v>3</v>
@@ -2688,7 +2685,7 @@
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B51">
         <v>3</v>
@@ -2720,7 +2717,7 @@
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B52">
         <v>3</v>
@@ -2752,7 +2749,7 @@
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B53">
         <v>3</v>
@@ -2784,7 +2781,7 @@
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B54">
         <v>4</v>
@@ -2814,18 +2811,18 @@
         <v>0</v>
       </c>
       <c r="L54" t="s">
+        <v>160</v>
+      </c>
+      <c r="M54" t="s">
         <v>161</v>
       </c>
-      <c r="M54" t="s">
+      <c r="N54" t="s">
         <v>162</v>
-      </c>
-      <c r="N54" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B55">
         <v>4</v>
@@ -2857,7 +2854,7 @@
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B56">
         <v>4</v>
@@ -2889,7 +2886,7 @@
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B57">
         <v>4</v>
@@ -2921,7 +2918,7 @@
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B58">
         <v>4</v>
@@ -2953,7 +2950,7 @@
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B59">
         <v>4</v>
@@ -2985,7 +2982,7 @@
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B60">
         <v>4</v>
@@ -3017,7 +3014,7 @@
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B61">
         <v>4</v>
@@ -3049,7 +3046,7 @@
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B62">
         <v>4</v>
@@ -3081,7 +3078,7 @@
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B63">
         <v>4</v>
@@ -3113,7 +3110,7 @@
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B64">
         <v>4</v>
@@ -3145,7 +3142,7 @@
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B65">
         <v>4</v>
@@ -3177,7 +3174,7 @@
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B66">
         <v>4</v>
@@ -3209,7 +3206,7 @@
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B67">
         <v>5</v>
@@ -3239,18 +3236,18 @@
         <v>0</v>
       </c>
       <c r="L67" t="s">
+        <v>136</v>
+      </c>
+      <c r="M67" t="s">
         <v>137</v>
       </c>
-      <c r="M67" t="s">
+      <c r="N67" t="s">
         <v>138</v>
-      </c>
-      <c r="N67" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B68">
         <v>5</v>
@@ -3280,18 +3277,18 @@
         <v>0</v>
       </c>
       <c r="L68" t="s">
+        <v>151</v>
+      </c>
+      <c r="M68" t="s">
         <v>152</v>
       </c>
-      <c r="M68" t="s">
+      <c r="N68" t="s">
         <v>153</v>
-      </c>
-      <c r="N68" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B69">
         <v>5</v>
@@ -3321,18 +3318,18 @@
         <v>0</v>
       </c>
       <c r="L69" t="s">
+        <v>157</v>
+      </c>
+      <c r="M69" t="s">
         <v>158</v>
       </c>
-      <c r="M69" t="s">
+      <c r="N69" t="s">
         <v>159</v>
-      </c>
-      <c r="N69" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B70">
         <v>5</v>
@@ -3364,7 +3361,7 @@
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B71">
         <v>5</v>
@@ -3396,7 +3393,7 @@
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B72">
         <v>5</v>
@@ -3428,7 +3425,7 @@
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B73">
         <v>5</v>
@@ -3460,7 +3457,7 @@
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B74">
         <v>5</v>
@@ -3492,7 +3489,7 @@
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B75">
         <v>5</v>
@@ -3524,7 +3521,7 @@
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B76">
         <v>5</v>
@@ -3556,7 +3553,7 @@
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B77">
         <v>5</v>
@@ -3588,7 +3585,7 @@
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B78">
         <v>5</v>
@@ -3620,7 +3617,7 @@
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B79">
         <v>5</v>
@@ -3652,7 +3649,7 @@
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B80">
         <v>6</v>
@@ -3682,18 +3679,18 @@
         <v>0</v>
       </c>
       <c r="L80" t="s">
+        <v>163</v>
+      </c>
+      <c r="M80" t="s">
         <v>164</v>
       </c>
-      <c r="M80" t="s">
+      <c r="N80" t="s">
         <v>165</v>
-      </c>
-      <c r="N80" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B81">
         <v>6</v>
@@ -3725,7 +3722,7 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B82">
         <v>6</v>
@@ -3757,7 +3754,7 @@
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B83">
         <v>6</v>
@@ -3789,7 +3786,7 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B84">
         <v>6</v>
@@ -3821,7 +3818,7 @@
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B85">
         <v>6</v>
@@ -3853,7 +3850,7 @@
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B86">
         <v>6</v>
@@ -3885,7 +3882,7 @@
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B87">
         <v>6</v>
@@ -3917,7 +3914,7 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B88">
         <v>6</v>
@@ -3949,7 +3946,7 @@
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B89">
         <v>6</v>
@@ -3981,7 +3978,7 @@
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B90">
         <v>6</v>
@@ -4013,7 +4010,7 @@
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B91">
         <v>6</v>
@@ -4045,7 +4042,7 @@
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B92">
         <v>6</v>
@@ -4077,7 +4074,7 @@
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B93">
         <v>7</v>
@@ -4109,7 +4106,7 @@
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B94">
         <v>7</v>
@@ -4141,7 +4138,7 @@
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B95">
         <v>7</v>
@@ -4173,7 +4170,7 @@
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B96">
         <v>7</v>
@@ -4205,7 +4202,7 @@
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B97">
         <v>7</v>
@@ -4237,7 +4234,7 @@
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B98">
         <v>7</v>
@@ -4269,7 +4266,7 @@
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B99">
         <v>7</v>
@@ -4301,7 +4298,7 @@
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B100">
         <v>7</v>
@@ -4333,7 +4330,7 @@
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B101">
         <v>7</v>
@@ -4363,18 +4360,18 @@
         <v>-20</v>
       </c>
       <c r="L101" t="s">
+        <v>172</v>
+      </c>
+      <c r="M101" t="s">
         <v>173</v>
       </c>
-      <c r="M101" t="s">
+      <c r="N101" t="s">
         <v>174</v>
-      </c>
-      <c r="N101" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B102">
         <v>7</v>
@@ -4406,7 +4403,7 @@
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B103">
         <v>7</v>
@@ -4438,7 +4435,7 @@
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B104">
         <v>7</v>
@@ -4470,7 +4467,7 @@
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B105">
         <v>7</v>
@@ -4502,7 +4499,7 @@
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B106">
         <v>8</v>
@@ -4532,18 +4529,18 @@
         <v>0</v>
       </c>
       <c r="L106" t="s">
+        <v>139</v>
+      </c>
+      <c r="M106" t="s">
         <v>140</v>
       </c>
-      <c r="M106" t="s">
+      <c r="N106" t="s">
         <v>141</v>
-      </c>
-      <c r="N106" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B107">
         <v>8</v>
@@ -4573,18 +4570,18 @@
         <v>0</v>
       </c>
       <c r="L107" t="s">
+        <v>142</v>
+      </c>
+      <c r="M107" t="s">
         <v>143</v>
       </c>
-      <c r="M107" t="s">
+      <c r="N107" t="s">
         <v>144</v>
-      </c>
-      <c r="N107" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B108">
         <v>8</v>
@@ -4616,7 +4613,7 @@
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B109">
         <v>8</v>
@@ -4648,7 +4645,7 @@
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B110">
         <v>8</v>
@@ -4680,7 +4677,7 @@
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B111">
         <v>8</v>
@@ -4712,7 +4709,7 @@
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B112">
         <v>8</v>
@@ -4744,7 +4741,7 @@
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B113">
         <v>8</v>
@@ -4776,7 +4773,7 @@
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B114">
         <v>8</v>
@@ -4808,7 +4805,7 @@
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B115">
         <v>8</v>
@@ -4840,7 +4837,7 @@
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B116">
         <v>8</v>
@@ -4872,7 +4869,7 @@
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B117">
         <v>8</v>
@@ -4904,7 +4901,7 @@
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B118">
         <v>8</v>
@@ -4957,7 +4954,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B1" t="s">
         <v>29</v>
@@ -4966,25 +4963,25 @@
         <v>30</v>
       </c>
       <c r="D1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E1" t="s">
         <v>180</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>181</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>182</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>183</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>184</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>185</v>
-      </c>
-      <c r="J1" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -9708,43 +9705,43 @@
   <sheetData>
     <row r="1" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D1" t="s">
         <v>187</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>188</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>189</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>190</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>191</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>192</v>
       </c>
-      <c r="I1" t="s">
-        <v>193</v>
-      </c>
       <c r="J1" t="s">
+        <v>195</v>
+      </c>
+      <c r="K1" t="s">
         <v>196</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>197</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>198</v>
-      </c>
-      <c r="M1" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -10044,7 +10041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1831AD9F-ED0A-47CF-B524-8603AB7A285B}">
   <dimension ref="A1:I78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -10055,16 +10052,16 @@
   <sheetData>
     <row r="1" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D1" t="s">
         <v>194</v>
-      </c>
-      <c r="C1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D1" t="s">
-        <v>195</v>
       </c>
       <c r="E1" t="s">
         <v>26</v>
@@ -10073,13 +10070,13 @@
         <v>27</v>
       </c>
       <c r="G1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H1" t="s">
         <v>28</v>
       </c>
       <c r="I1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
InnerGradeTable 에 amplifyRandomGold|Int 컬럼 추가 OptionTable 에 amplifyGold|Int 컬럼 제거
</commit_message>
<xml_diff>
--- a/Excel/Equip.xlsx
+++ b/Excel/Equip.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553C17D1-E3D3-4331-AB8E-E82F0BA4B6E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36EBF308-9FC9-4CBA-AA7F-17ECFF2936C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{744FAB8B-2B4C-47C4-9B52-EAF29B7E3396}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{744FAB8B-2B4C-47C4-9B52-EAF29B7E3396}"/>
   </bookViews>
   <sheets>
     <sheet name="EquipTable" sheetId="1" r:id="rId1"/>
@@ -727,9 +727,6 @@
     <t>transmuteRandomGold|Int</t>
   </si>
   <si>
-    <t>amplifyGold|Int</t>
-  </si>
-  <si>
     <t>transferGold|Int</t>
   </si>
   <si>
@@ -758,6 +755,9 @@
   </si>
   <si>
     <t>innerGradeSixAmount|Float</t>
+  </si>
+  <si>
+    <t>amplifyRandomGold|Int</t>
   </si>
 </sst>
 </file>
@@ -9608,13 +9608,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A82CFE85-E5BF-4028-97DD-0FD3D41C3DD1}">
-  <dimension ref="A1:AC8"/>
+  <dimension ref="A1:AD8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:29" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>178</v>
       </c>
@@ -9697,13 +9697,16 @@
         <v>228</v>
       </c>
       <c r="AB1" t="s">
+        <v>240</v>
+      </c>
+      <c r="AC1" t="s">
         <v>229</v>
       </c>
-      <c r="AC1" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -9780,13 +9783,16 @@
         <v>1000</v>
       </c>
       <c r="AB2">
+        <v>200</v>
+      </c>
+      <c r="AC2">
         <v>750</v>
       </c>
-      <c r="AC2">
+      <c r="AD2">
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -9863,13 +9869,16 @@
         <v>2000</v>
       </c>
       <c r="AB3">
+        <v>400</v>
+      </c>
+      <c r="AC3">
         <v>1500</v>
       </c>
-      <c r="AC3">
+      <c r="AD3">
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -9946,13 +9955,16 @@
         <v>3000</v>
       </c>
       <c r="AB4">
+        <v>600</v>
+      </c>
+      <c r="AC4">
         <v>2250</v>
       </c>
-      <c r="AC4">
+      <c r="AD4">
         <v>1500</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -10029,13 +10041,16 @@
         <v>4000</v>
       </c>
       <c r="AB5">
+        <v>800</v>
+      </c>
+      <c r="AC5">
         <v>3000</v>
       </c>
-      <c r="AC5">
+      <c r="AD5">
         <v>2000</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -10115,13 +10130,16 @@
         <v>5000</v>
       </c>
       <c r="AB6">
+        <v>1000</v>
+      </c>
+      <c r="AC6">
         <v>3750</v>
       </c>
-      <c r="AC6">
+      <c r="AD6">
         <v>2500</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -10201,13 +10219,16 @@
         <v>5000</v>
       </c>
       <c r="AB7">
+        <v>1000</v>
+      </c>
+      <c r="AC7">
         <v>3750</v>
       </c>
-      <c r="AC7">
+      <c r="AD7">
         <v>2500</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -10287,9 +10308,12 @@
         <v>5000</v>
       </c>
       <c r="AB8">
+        <v>1000</v>
+      </c>
+      <c r="AC8">
         <v>3750</v>
       </c>
-      <c r="AC8">
+      <c r="AD8">
         <v>2500</v>
       </c>
     </row>
@@ -10301,10 +10325,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1831AD9F-ED0A-47CF-B524-8603AB7A285B}">
-  <dimension ref="A1:O78"/>
+  <dimension ref="A1:N78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O2" sqref="O2:O8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -10312,7 +10336,7 @@
     <col min="1" max="1" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -10355,11 +10379,8 @@
       <c r="N1" t="s">
         <v>207</v>
       </c>
-      <c r="O1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -10390,11 +10411,8 @@
       <c r="L2">
         <v>0</v>
       </c>
-      <c r="O2">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
@@ -10425,11 +10443,8 @@
       <c r="L3">
         <v>0</v>
       </c>
-      <c r="O3">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0</v>
       </c>
@@ -10460,11 +10475,8 @@
       <c r="L4">
         <v>0</v>
       </c>
-      <c r="O4">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0</v>
       </c>
@@ -10495,11 +10507,8 @@
       <c r="L5">
         <v>0</v>
       </c>
-      <c r="O5">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0</v>
       </c>
@@ -10536,11 +10545,8 @@
       <c r="M6">
         <v>-20</v>
       </c>
-      <c r="O6">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0</v>
       </c>
@@ -10577,11 +10583,8 @@
       <c r="M7">
         <v>-10</v>
       </c>
-      <c r="O7">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0</v>
       </c>
@@ -10618,11 +10621,8 @@
       <c r="M8">
         <v>-5</v>
       </c>
-      <c r="O8">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0</v>
       </c>
@@ -10653,11 +10653,8 @@
       <c r="L9">
         <v>0</v>
       </c>
-      <c r="O9">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>0</v>
       </c>
@@ -10688,11 +10685,8 @@
       <c r="L10">
         <v>0</v>
       </c>
-      <c r="O10">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>0</v>
       </c>
@@ -10723,11 +10717,8 @@
       <c r="L11">
         <v>0</v>
       </c>
-      <c r="O11">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>0</v>
       </c>
@@ -10758,11 +10749,8 @@
       <c r="L12">
         <v>0</v>
       </c>
-      <c r="O12">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>0</v>
       </c>
@@ -10799,11 +10787,8 @@
       <c r="M13">
         <v>-20</v>
       </c>
-      <c r="O13">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>0</v>
       </c>
@@ -10840,11 +10825,8 @@
       <c r="M14">
         <v>-10</v>
       </c>
-      <c r="O14">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>0</v>
       </c>
@@ -10881,11 +10863,8 @@
       <c r="M15">
         <v>-5</v>
       </c>
-      <c r="O15">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>0</v>
       </c>
@@ -10916,11 +10895,8 @@
       <c r="L16">
         <v>0</v>
       </c>
-      <c r="O16">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>0</v>
       </c>
@@ -10951,11 +10927,8 @@
       <c r="L17">
         <v>0</v>
       </c>
-      <c r="O17">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>0</v>
       </c>
@@ -10986,11 +10959,8 @@
       <c r="L18">
         <v>0</v>
       </c>
-      <c r="O18">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>0</v>
       </c>
@@ -11021,11 +10991,8 @@
       <c r="L19">
         <v>0</v>
       </c>
-      <c r="O19">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>0</v>
       </c>
@@ -11062,11 +11029,8 @@
       <c r="M20">
         <v>-20</v>
       </c>
-      <c r="O20">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>0</v>
       </c>
@@ -11103,11 +11067,8 @@
       <c r="M21">
         <v>-10</v>
       </c>
-      <c r="O21">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>0</v>
       </c>
@@ -11144,11 +11105,8 @@
       <c r="M22">
         <v>-5</v>
       </c>
-      <c r="O22">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>0</v>
       </c>
@@ -11179,11 +11137,8 @@
       <c r="L23">
         <v>0</v>
       </c>
-      <c r="O23">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>0</v>
       </c>
@@ -11214,11 +11169,8 @@
       <c r="L24">
         <v>0</v>
       </c>
-      <c r="O24">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>0</v>
       </c>
@@ -11249,11 +11201,8 @@
       <c r="L25">
         <v>0</v>
       </c>
-      <c r="O25">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>0</v>
       </c>
@@ -11284,11 +11233,8 @@
       <c r="L26">
         <v>0</v>
       </c>
-      <c r="O26">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>0</v>
       </c>
@@ -11325,11 +11271,8 @@
       <c r="M27">
         <v>-20</v>
       </c>
-      <c r="O27">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>0</v>
       </c>
@@ -11366,11 +11309,8 @@
       <c r="M28">
         <v>-10</v>
       </c>
-      <c r="O28">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>0</v>
       </c>
@@ -11407,11 +11347,8 @@
       <c r="M29">
         <v>-5</v>
       </c>
-      <c r="O29">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>0</v>
       </c>
@@ -11442,11 +11379,8 @@
       <c r="L30">
         <v>0</v>
       </c>
-      <c r="O30">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>0</v>
       </c>
@@ -11477,11 +11411,8 @@
       <c r="L31">
         <v>0</v>
       </c>
-      <c r="O31">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>0</v>
       </c>
@@ -11512,11 +11443,8 @@
       <c r="L32">
         <v>0</v>
       </c>
-      <c r="O32">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>0</v>
       </c>
@@ -11547,11 +11475,8 @@
       <c r="L33">
         <v>0</v>
       </c>
-      <c r="O33">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>0</v>
       </c>
@@ -11588,11 +11513,8 @@
       <c r="M34">
         <v>-20</v>
       </c>
-      <c r="O34">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>0</v>
       </c>
@@ -11629,11 +11551,8 @@
       <c r="M35">
         <v>-10</v>
       </c>
-      <c r="O35">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>0</v>
       </c>
@@ -11670,11 +11589,8 @@
       <c r="M36">
         <v>-5</v>
       </c>
-      <c r="O36">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>0</v>
       </c>
@@ -11705,11 +11621,8 @@
       <c r="L37">
         <v>0</v>
       </c>
-      <c r="O37">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>0</v>
       </c>
@@ -11740,11 +11653,8 @@
       <c r="L38">
         <v>0</v>
       </c>
-      <c r="O38">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>0</v>
       </c>
@@ -11775,11 +11685,8 @@
       <c r="L39">
         <v>0</v>
       </c>
-      <c r="O39">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>0</v>
       </c>
@@ -11810,11 +11717,8 @@
       <c r="L40">
         <v>0</v>
       </c>
-      <c r="O40">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>0</v>
       </c>
@@ -11851,11 +11755,8 @@
       <c r="M41">
         <v>-20</v>
       </c>
-      <c r="O41">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>0</v>
       </c>
@@ -11892,11 +11793,8 @@
       <c r="M42">
         <v>-10</v>
       </c>
-      <c r="O42">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>0</v>
       </c>
@@ -11933,11 +11831,8 @@
       <c r="M43">
         <v>-5</v>
       </c>
-      <c r="O43">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>1</v>
       </c>
@@ -11968,11 +11863,8 @@
       <c r="L44">
         <v>0</v>
       </c>
-      <c r="O44">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>1</v>
       </c>
@@ -12003,11 +11895,8 @@
       <c r="L45">
         <v>0</v>
       </c>
-      <c r="O45">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>1</v>
       </c>
@@ -12038,11 +11927,8 @@
       <c r="L46">
         <v>0</v>
       </c>
-      <c r="O46">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>1</v>
       </c>
@@ -12073,11 +11959,8 @@
       <c r="L47">
         <v>0</v>
       </c>
-      <c r="O47">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>1</v>
       </c>
@@ -12114,11 +11997,8 @@
       <c r="M48">
         <v>-20</v>
       </c>
-      <c r="O48">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>1</v>
       </c>
@@ -12155,11 +12035,8 @@
       <c r="M49">
         <v>-10</v>
       </c>
-      <c r="O49">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>1</v>
       </c>
@@ -12196,11 +12073,8 @@
       <c r="M50">
         <v>-5</v>
       </c>
-      <c r="O50">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>1</v>
       </c>
@@ -12231,11 +12105,8 @@
       <c r="L51">
         <v>0</v>
       </c>
-      <c r="O51">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>1</v>
       </c>
@@ -12266,11 +12137,8 @@
       <c r="L52">
         <v>0</v>
       </c>
-      <c r="O52">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>1</v>
       </c>
@@ -12301,11 +12169,8 @@
       <c r="L53">
         <v>0</v>
       </c>
-      <c r="O53">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>1</v>
       </c>
@@ -12336,11 +12201,8 @@
       <c r="L54">
         <v>0</v>
       </c>
-      <c r="O54">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>1</v>
       </c>
@@ -12377,11 +12239,8 @@
       <c r="M55">
         <v>-20</v>
       </c>
-      <c r="O55">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>1</v>
       </c>
@@ -12418,11 +12277,8 @@
       <c r="M56">
         <v>-10</v>
       </c>
-      <c r="O56">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>1</v>
       </c>
@@ -12459,11 +12315,8 @@
       <c r="M57">
         <v>-5</v>
       </c>
-      <c r="O57">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>1</v>
       </c>
@@ -12494,11 +12347,8 @@
       <c r="L58">
         <v>0</v>
       </c>
-      <c r="O58">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>1</v>
       </c>
@@ -12529,11 +12379,8 @@
       <c r="L59">
         <v>0</v>
       </c>
-      <c r="O59">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>1</v>
       </c>
@@ -12564,11 +12411,8 @@
       <c r="L60">
         <v>0</v>
       </c>
-      <c r="O60">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>1</v>
       </c>
@@ -12599,11 +12443,8 @@
       <c r="L61">
         <v>0</v>
       </c>
-      <c r="O61">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>1</v>
       </c>
@@ -12640,11 +12481,8 @@
       <c r="M62">
         <v>-20</v>
       </c>
-      <c r="O62">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>1</v>
       </c>
@@ -12681,11 +12519,8 @@
       <c r="M63">
         <v>-10</v>
       </c>
-      <c r="O63">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>1</v>
       </c>
@@ -12722,11 +12557,8 @@
       <c r="M64">
         <v>-5</v>
       </c>
-      <c r="O64">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>1</v>
       </c>
@@ -12757,11 +12589,8 @@
       <c r="L65">
         <v>0</v>
       </c>
-      <c r="O65">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>1</v>
       </c>
@@ -12792,11 +12621,8 @@
       <c r="L66">
         <v>0</v>
       </c>
-      <c r="O66">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>1</v>
       </c>
@@ -12827,11 +12653,8 @@
       <c r="L67">
         <v>0</v>
       </c>
-      <c r="O67">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>1</v>
       </c>
@@ -12862,11 +12685,8 @@
       <c r="L68">
         <v>0</v>
       </c>
-      <c r="O68">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>1</v>
       </c>
@@ -12903,11 +12723,8 @@
       <c r="M69">
         <v>-20</v>
       </c>
-      <c r="O69">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>1</v>
       </c>
@@ -12944,11 +12761,8 @@
       <c r="M70">
         <v>-10</v>
       </c>
-      <c r="O70">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>1</v>
       </c>
@@ -12985,11 +12799,8 @@
       <c r="M71">
         <v>-5</v>
       </c>
-      <c r="O71">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>1</v>
       </c>
@@ -13020,11 +12831,8 @@
       <c r="L72">
         <v>0</v>
       </c>
-      <c r="O72">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>1</v>
       </c>
@@ -13055,11 +12863,8 @@
       <c r="L73">
         <v>0</v>
       </c>
-      <c r="O73">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>1</v>
       </c>
@@ -13090,11 +12895,8 @@
       <c r="L74">
         <v>0</v>
       </c>
-      <c r="O74">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>1</v>
       </c>
@@ -13125,11 +12927,8 @@
       <c r="L75">
         <v>0</v>
       </c>
-      <c r="O75">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>1</v>
       </c>
@@ -13166,11 +12965,8 @@
       <c r="M76">
         <v>-20</v>
       </c>
-      <c r="O76">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>1</v>
       </c>
@@ -13207,11 +13003,8 @@
       <c r="M77">
         <v>-10</v>
       </c>
-      <c r="O77">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>1</v>
       </c>
@@ -13247,9 +13040,6 @@
       </c>
       <c r="M78">
         <v>-5</v>
-      </c>
-      <c r="O78">
-        <v>1000</v>
       </c>
     </row>
   </sheetData>
@@ -13262,7 +13052,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07F218ED-5790-4589-A336-D604CD6FE4FD}">
   <dimension ref="A1:K148"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -13276,31 +13066,31 @@
         <v>29</v>
       </c>
       <c r="C1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D1" t="s">
         <v>232</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>233</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>234</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>235</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>236</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>237</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>238</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>239</v>
-      </c>
-      <c r="K1" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
신규 검 Equip5201 추가
</commit_message>
<xml_diff>
--- a/Excel/Equip.xlsx
+++ b/Excel/Equip.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B7CF4F-2D51-4F8D-94EF-813AD89560BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E595D3-DDEE-45D3-936E-130545163DE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{744FAB8B-2B4C-47C4-9B52-EAF29B7E3396}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{744FAB8B-2B4C-47C4-9B52-EAF29B7E3396}"/>
   </bookViews>
   <sheets>
     <sheet name="EquipTable" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="253">
   <si>
     <t>Equip0001</t>
   </si>
@@ -785,6 +785,15 @@
   </si>
   <si>
     <t>EquipName_StylizedAxe</t>
+  </si>
+  <si>
+    <t>StylizedSword</t>
+  </si>
+  <si>
+    <t>Shot_StylizedSword</t>
+  </si>
+  <si>
+    <t>EquipName_StylizedSword</t>
   </si>
 </sst>
 </file>
@@ -3436,6 +3445,15 @@
       <c r="I71">
         <v>0</v>
       </c>
+      <c r="L71" t="s">
+        <v>250</v>
+      </c>
+      <c r="M71" t="s">
+        <v>251</v>
+      </c>
+      <c r="N71" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A72" t="s">

</xml_diff>

<commit_message>
신규 검 추가 Equip5202
</commit_message>
<xml_diff>
--- a/Excel/Equip.xlsx
+++ b/Excel/Equip.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1CFE3A7-A15A-453A-A112-8DF9901EFCA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E7FE4D-3488-4C84-A695-20489C817614}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{744FAB8B-2B4C-47C4-9B52-EAF29B7E3396}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="259">
   <si>
     <t>Equip0001</t>
   </si>
@@ -803,6 +803,15 @@
   </si>
   <si>
     <t>EquipName_LowPolyHammer</t>
+  </si>
+  <si>
+    <t>SevenBroadSword</t>
+  </si>
+  <si>
+    <t>Shot_SevenBroadSword</t>
+  </si>
+  <si>
+    <t>EquipName_SevenBroadSword</t>
   </si>
 </sst>
 </file>
@@ -1171,7 +1180,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{314FDFEB-84DC-4FDB-9708-1D7DBC9715D5}">
   <dimension ref="A1:N118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -3500,6 +3509,15 @@
       </c>
       <c r="I72">
         <v>0</v>
+      </c>
+      <c r="L72" t="s">
+        <v>256</v>
+      </c>
+      <c r="M72" t="s">
+        <v>257</v>
+      </c>
+      <c r="N72" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
무기 헤비 시리즈 5종 추가 Equip4101, Equip4102, Equip0102, Equip0201, Equip8102
</commit_message>
<xml_diff>
--- a/Excel/Equip.xlsx
+++ b/Excel/Equip.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6DE15E2-267C-4504-BAC6-B26B0A66FA1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732C246B-2D43-4527-9009-E1904E32884B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{744FAB8B-2B4C-47C4-9B52-EAF29B7E3396}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{744FAB8B-2B4C-47C4-9B52-EAF29B7E3396}"/>
   </bookViews>
   <sheets>
     <sheet name="EquipTable" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="290">
   <si>
     <t>Equip0001</t>
   </si>
@@ -862,6 +862,51 @@
   </si>
   <si>
     <t>EquipName_FullMetalSword</t>
+  </si>
+  <si>
+    <t>HeavyAxe</t>
+  </si>
+  <si>
+    <t>Shot_HeavyAxe</t>
+  </si>
+  <si>
+    <t>EquipName_HeavyAxe</t>
+  </si>
+  <si>
+    <t>HeavySkullAxe</t>
+  </si>
+  <si>
+    <t>Shot_HeavySkullAxe</t>
+  </si>
+  <si>
+    <t>EquipName_HeavySkullAxe</t>
+  </si>
+  <si>
+    <t>HeavyHammer</t>
+  </si>
+  <si>
+    <t>Shot_HeavyHammer</t>
+  </si>
+  <si>
+    <t>EquipName_HeavyHammer</t>
+  </si>
+  <si>
+    <t>HeavyMace</t>
+  </si>
+  <si>
+    <t>Shot_HeavyMace</t>
+  </si>
+  <si>
+    <t>EquipName_HeavyMace</t>
+  </si>
+  <si>
+    <t>HeavyDarkSword</t>
+  </si>
+  <si>
+    <t>Shot_HeavyDarkSword</t>
+  </si>
+  <si>
+    <t>EquipName_HeavyDarkSword</t>
   </si>
 </sst>
 </file>
@@ -1473,6 +1518,27 @@
       <c r="I5">
         <v>0</v>
       </c>
+      <c r="L5" t="s">
+        <v>275</v>
+      </c>
+      <c r="M5" t="s">
+        <v>276</v>
+      </c>
+      <c r="N5" t="s">
+        <v>277</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>2</v>
+      </c>
+      <c r="Q5">
+        <v>10</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -1502,6 +1568,27 @@
       <c r="I6">
         <v>0</v>
       </c>
+      <c r="L6" t="s">
+        <v>278</v>
+      </c>
+      <c r="M6" t="s">
+        <v>279</v>
+      </c>
+      <c r="N6" t="s">
+        <v>280</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>2</v>
+      </c>
+      <c r="Q6">
+        <v>10</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -3201,6 +3288,27 @@
       <c r="I56">
         <v>0</v>
       </c>
+      <c r="L56" t="s">
+        <v>281</v>
+      </c>
+      <c r="M56" t="s">
+        <v>282</v>
+      </c>
+      <c r="N56" t="s">
+        <v>283</v>
+      </c>
+      <c r="O56">
+        <v>1</v>
+      </c>
+      <c r="P56">
+        <v>3</v>
+      </c>
+      <c r="Q56">
+        <v>1</v>
+      </c>
+      <c r="R56">
+        <v>1</v>
+      </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
@@ -3230,6 +3338,27 @@
       <c r="I57">
         <v>0</v>
       </c>
+      <c r="L57" t="s">
+        <v>284</v>
+      </c>
+      <c r="M57" t="s">
+        <v>285</v>
+      </c>
+      <c r="N57" t="s">
+        <v>286</v>
+      </c>
+      <c r="O57">
+        <v>1</v>
+      </c>
+      <c r="P57">
+        <v>3</v>
+      </c>
+      <c r="Q57">
+        <v>1</v>
+      </c>
+      <c r="R57">
+        <v>1</v>
+      </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
@@ -5049,6 +5178,27 @@
       </c>
       <c r="I109">
         <v>0</v>
+      </c>
+      <c r="L109" t="s">
+        <v>287</v>
+      </c>
+      <c r="M109" t="s">
+        <v>288</v>
+      </c>
+      <c r="N109" t="s">
+        <v>289</v>
+      </c>
+      <c r="O109">
+        <v>1</v>
+      </c>
+      <c r="P109">
+        <v>4</v>
+      </c>
+      <c r="Q109">
+        <v>1</v>
+      </c>
+      <c r="R109">
+        <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:18" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
신규 밀리 무기 시리즈 3개 추가 Equip0302, Equip4201, Equip5301
</commit_message>
<xml_diff>
--- a/Excel/Equip.xlsx
+++ b/Excel/Equip.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0CB18C3-1B0A-40CF-8192-B3CFCD9B0C5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB6A2C8-24DD-46B8-A9FE-E35DA6FF66C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{744FAB8B-2B4C-47C4-9B52-EAF29B7E3396}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{744FAB8B-2B4C-47C4-9B52-EAF29B7E3396}"/>
   </bookViews>
   <sheets>
     <sheet name="EquipTable" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="302">
   <si>
     <t>Equip0001</t>
   </si>
@@ -916,6 +916,33 @@
   </si>
   <si>
     <t>EquipName_StAxe</t>
+  </si>
+  <si>
+    <t>MeleeAxe</t>
+  </si>
+  <si>
+    <t>Shot_MeleeAxe</t>
+  </si>
+  <si>
+    <t>EquipName_MeleeAxe</t>
+  </si>
+  <si>
+    <t>MeleeHammer</t>
+  </si>
+  <si>
+    <t>Shot_MeleeHammer</t>
+  </si>
+  <si>
+    <t>EquipName_MeleeHammer</t>
+  </si>
+  <si>
+    <t>MeleeMachete</t>
+  </si>
+  <si>
+    <t>Shot_MeleeMachete</t>
+  </si>
+  <si>
+    <t>EquipName_MeleeMachete</t>
   </si>
 </sst>
 </file>
@@ -1727,6 +1754,27 @@
       <c r="I9">
         <v>0</v>
       </c>
+      <c r="L9" t="s">
+        <v>293</v>
+      </c>
+      <c r="M9" t="s">
+        <v>294</v>
+      </c>
+      <c r="N9" t="s">
+        <v>295</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>3</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+      <c r="R9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -3418,6 +3466,27 @@
       <c r="I58">
         <v>0</v>
       </c>
+      <c r="L58" t="s">
+        <v>296</v>
+      </c>
+      <c r="M58" t="s">
+        <v>297</v>
+      </c>
+      <c r="N58" t="s">
+        <v>298</v>
+      </c>
+      <c r="O58">
+        <v>1</v>
+      </c>
+      <c r="P58">
+        <v>3</v>
+      </c>
+      <c r="Q58">
+        <v>1</v>
+      </c>
+      <c r="R58">
+        <v>1</v>
+      </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
@@ -3993,6 +4062,27 @@
       </c>
       <c r="I73">
         <v>0</v>
+      </c>
+      <c r="L73" t="s">
+        <v>299</v>
+      </c>
+      <c r="M73" t="s">
+        <v>300</v>
+      </c>
+      <c r="N73" t="s">
+        <v>301</v>
+      </c>
+      <c r="O73">
+        <v>1</v>
+      </c>
+      <c r="P73">
+        <v>3</v>
+      </c>
+      <c r="Q73">
+        <v>1</v>
+      </c>
+      <c r="R73">
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
총 3자루 추가 Equip6002, Equip6101, Equip6301
</commit_message>
<xml_diff>
--- a/Excel/Equip.xlsx
+++ b/Excel/Equip.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA1B8CB2-15CE-4EBE-87C4-5ABA816BDFD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74675751-1EDB-4CFF-A10B-E1989CE41765}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{744FAB8B-2B4C-47C4-9B52-EAF29B7E3396}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="320">
   <si>
     <t>Equip0001</t>
   </si>
@@ -970,6 +970,33 @@
   </si>
   <si>
     <t>EquipName_MorfusSword</t>
+  </si>
+  <si>
+    <t>SMG28</t>
+  </si>
+  <si>
+    <t>Shot_SMG28</t>
+  </si>
+  <si>
+    <t>EquipName_SMG28</t>
+  </si>
+  <si>
+    <t>SMG31</t>
+  </si>
+  <si>
+    <t>Shot_SMG31</t>
+  </si>
+  <si>
+    <t>EquipName_SMG31</t>
+  </si>
+  <si>
+    <t>SMG30</t>
+  </si>
+  <si>
+    <t>Shot_SMG30</t>
+  </si>
+  <si>
+    <t>EquipName_SMG30</t>
   </si>
 </sst>
 </file>
@@ -4421,6 +4448,27 @@
       <c r="I81">
         <v>0</v>
       </c>
+      <c r="L81" t="s">
+        <v>311</v>
+      </c>
+      <c r="M81" t="s">
+        <v>312</v>
+      </c>
+      <c r="N81" t="s">
+        <v>313</v>
+      </c>
+      <c r="O81">
+        <v>1</v>
+      </c>
+      <c r="P81">
+        <v>3</v>
+      </c>
+      <c r="Q81">
+        <v>1</v>
+      </c>
+      <c r="R81">
+        <v>1</v>
+      </c>
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
@@ -4450,6 +4498,27 @@
       <c r="I82">
         <v>0</v>
       </c>
+      <c r="L82" t="s">
+        <v>314</v>
+      </c>
+      <c r="M82" t="s">
+        <v>315</v>
+      </c>
+      <c r="N82" t="s">
+        <v>316</v>
+      </c>
+      <c r="O82">
+        <v>1</v>
+      </c>
+      <c r="P82">
+        <v>3</v>
+      </c>
+      <c r="Q82">
+        <v>1</v>
+      </c>
+      <c r="R82">
+        <v>1</v>
+      </c>
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
@@ -4565,6 +4634,27 @@
       </c>
       <c r="I86">
         <v>0</v>
+      </c>
+      <c r="L86" t="s">
+        <v>317</v>
+      </c>
+      <c r="M86" t="s">
+        <v>318</v>
+      </c>
+      <c r="N86" t="s">
+        <v>319</v>
+      </c>
+      <c r="O86">
+        <v>1</v>
+      </c>
+      <c r="P86">
+        <v>3</v>
+      </c>
+      <c r="Q86">
+        <v>1</v>
+      </c>
+      <c r="R86">
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:18" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Equip2401 Equip4301 Equip0403 신규 엘프 시리즈 무기 추가
</commit_message>
<xml_diff>
--- a/Excel/Equip.xlsx
+++ b/Excel/Equip.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28EF39C9-FB99-4D50-A81D-F66E618287DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2A1333-9B19-4CE2-8A89-46315E49EDE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{744FAB8B-2B4C-47C4-9B52-EAF29B7E3396}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="356">
   <si>
     <t>Equip0001</t>
   </si>
@@ -1078,6 +1078,33 @@
   </si>
   <si>
     <t>EquipName_SunSword</t>
+  </si>
+  <si>
+    <t>ElvenBow</t>
+  </si>
+  <si>
+    <t>ElvenAxe</t>
+  </si>
+  <si>
+    <t>Shot_ElvenAxe</t>
+  </si>
+  <si>
+    <t>EquipName_ElvenAxe</t>
+  </si>
+  <si>
+    <t>Shot_ElvenBow</t>
+  </si>
+  <si>
+    <t>EquipName_ElvenBow</t>
+  </si>
+  <si>
+    <t>ElvenHammer</t>
+  </si>
+  <si>
+    <t>Shot_ElvenHammer</t>
+  </si>
+  <si>
+    <t>EquipName_ElvenHammer</t>
   </si>
 </sst>
 </file>
@@ -1446,7 +1473,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{314FDFEB-84DC-4FDB-9708-1D7DBC9715D5}">
   <dimension ref="A1:R118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2046,6 +2075,27 @@
       <c r="J12">
         <v>-10</v>
       </c>
+      <c r="L12" t="s">
+        <v>348</v>
+      </c>
+      <c r="M12" t="s">
+        <v>349</v>
+      </c>
+      <c r="N12" t="s">
+        <v>350</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>3</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -2871,6 +2921,27 @@
       <c r="J36">
         <v>-20</v>
       </c>
+      <c r="L36" t="s">
+        <v>347</v>
+      </c>
+      <c r="M36" t="s">
+        <v>351</v>
+      </c>
+      <c r="N36" t="s">
+        <v>352</v>
+      </c>
+      <c r="O36">
+        <v>1</v>
+      </c>
+      <c r="P36">
+        <v>4</v>
+      </c>
+      <c r="Q36">
+        <v>1</v>
+      </c>
+      <c r="R36">
+        <v>1</v>
+      </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
@@ -3782,6 +3853,27 @@
       </c>
       <c r="I60">
         <v>0</v>
+      </c>
+      <c r="L60" t="s">
+        <v>353</v>
+      </c>
+      <c r="M60" t="s">
+        <v>354</v>
+      </c>
+      <c r="N60" t="s">
+        <v>355</v>
+      </c>
+      <c r="O60">
+        <v>1</v>
+      </c>
+      <c r="P60">
+        <v>3</v>
+      </c>
+      <c r="Q60">
+        <v>1</v>
+      </c>
+      <c r="R60">
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Equip6202, Equip6201 무기 2개 추가
</commit_message>
<xml_diff>
--- a/Excel/Equip.xlsx
+++ b/Excel/Equip.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBAED25C-23F5-4DFE-9A82-5A589AA2B87C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3BBD5B8-B272-4B2E-B042-01FE4C7116DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{744FAB8B-2B4C-47C4-9B52-EAF29B7E3396}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="380">
   <si>
     <t>Equip0001</t>
   </si>
@@ -1159,6 +1159,24 @@
   </si>
   <si>
     <t>EquipName_FantasyShield</t>
+  </si>
+  <si>
+    <t>PetalShotgun</t>
+  </si>
+  <si>
+    <t>Shot_PetalShotgun</t>
+  </si>
+  <si>
+    <t>EquipName_PetalShotgun</t>
+  </si>
+  <si>
+    <t>BubbleBlaster</t>
+  </si>
+  <si>
+    <t>Shot_BubbleBlaster</t>
+  </si>
+  <si>
+    <t>EquipName_BubbleBlaster</t>
   </si>
 </sst>
 </file>
@@ -1527,9 +1545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{314FDFEB-84DC-4FDB-9708-1D7DBC9715D5}">
   <dimension ref="A1:R118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4991,6 +5007,27 @@
       <c r="I84">
         <v>0</v>
       </c>
+      <c r="L84" t="s">
+        <v>374</v>
+      </c>
+      <c r="M84" t="s">
+        <v>375</v>
+      </c>
+      <c r="N84" t="s">
+        <v>376</v>
+      </c>
+      <c r="O84">
+        <v>1</v>
+      </c>
+      <c r="P84">
+        <v>3</v>
+      </c>
+      <c r="Q84">
+        <v>1</v>
+      </c>
+      <c r="R84">
+        <v>1</v>
+      </c>
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
@@ -5019,6 +5056,27 @@
       </c>
       <c r="I85">
         <v>0</v>
+      </c>
+      <c r="L85" t="s">
+        <v>377</v>
+      </c>
+      <c r="M85" t="s">
+        <v>378</v>
+      </c>
+      <c r="N85" t="s">
+        <v>379</v>
+      </c>
+      <c r="O85">
+        <v>1</v>
+      </c>
+      <c r="P85">
+        <v>3</v>
+      </c>
+      <c r="Q85">
+        <v>1</v>
+      </c>
+      <c r="R85">
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Equip6302 신규 총 추가
</commit_message>
<xml_diff>
--- a/Excel/Equip.xlsx
+++ b/Excel/Equip.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4ED771-DF3C-4EC5-842B-F79F9E25A32C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D2C2F7B-4C96-4B91-B09C-49B5FB61F007}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{744FAB8B-2B4C-47C4-9B52-EAF29B7E3396}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="398">
   <si>
     <t>Equip0001</t>
   </si>
@@ -1222,6 +1222,15 @@
   </si>
   <si>
     <t>EquipName_HeavySword</t>
+  </si>
+  <si>
+    <t>SciFiGun</t>
+  </si>
+  <si>
+    <t>Shot_SciFiGun</t>
+  </si>
+  <si>
+    <t>EquipName_SciFiGun</t>
   </si>
 </sst>
 </file>
@@ -5267,6 +5276,27 @@
       <c r="I87">
         <v>0</v>
       </c>
+      <c r="L87" t="s">
+        <v>395</v>
+      </c>
+      <c r="M87" t="s">
+        <v>396</v>
+      </c>
+      <c r="N87" t="s">
+        <v>397</v>
+      </c>
+      <c r="O87">
+        <v>1</v>
+      </c>
+      <c r="P87">
+        <v>3</v>
+      </c>
+      <c r="Q87">
+        <v>1</v>
+      </c>
+      <c r="R87">
+        <v>1</v>
+      </c>
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A88" t="s">

</xml_diff>

<commit_message>
Equip6401 신규 총 추가
</commit_message>
<xml_diff>
--- a/Excel/Equip.xlsx
+++ b/Excel/Equip.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D2C2F7B-4C96-4B91-B09C-49B5FB61F007}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A449D13-92D3-467A-9B00-A55A9ABEB1DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{744FAB8B-2B4C-47C4-9B52-EAF29B7E3396}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{744FAB8B-2B4C-47C4-9B52-EAF29B7E3396}"/>
   </bookViews>
   <sheets>
     <sheet name="EquipTable" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="401">
   <si>
     <t>Equip0001</t>
   </si>
@@ -1231,6 +1231,15 @@
   </si>
   <si>
     <t>EquipName_SciFiGun</t>
+  </si>
+  <si>
+    <t>RayRevolver</t>
+  </si>
+  <si>
+    <t>Shot_RayRevolver</t>
+  </si>
+  <si>
+    <t>EquipName_RayRevolver</t>
   </si>
 </sst>
 </file>
@@ -1599,8 +1608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{314FDFEB-84DC-4FDB-9708-1D7DBC9715D5}">
   <dimension ref="A1:R118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="A88" sqref="A88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5328,6 +5337,27 @@
       </c>
       <c r="J88">
         <v>-20</v>
+      </c>
+      <c r="L88" t="s">
+        <v>398</v>
+      </c>
+      <c r="M88" t="s">
+        <v>399</v>
+      </c>
+      <c r="N88" t="s">
+        <v>400</v>
+      </c>
+      <c r="O88">
+        <v>1</v>
+      </c>
+      <c r="P88">
+        <v>3</v>
+      </c>
+      <c r="Q88">
+        <v>1</v>
+      </c>
+      <c r="R88">
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:18" x14ac:dyDescent="0.3">

</xml_diff>